<commit_message>
add go giff to readme
</commit_message>
<xml_diff>
--- a/conditionFiles/instructions.xlsx
+++ b/conditionFiles/instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\PycharmProjects\OSARI_private\conditionFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Documents\GitHub\OSARI-1\conditionFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6931F62-CEEB-49C9-B4F3-B917764BC6F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5274111C-BA24-4B28-ABAC-899D4163416E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C4BCA8AB-96B2-4D72-9643-B068FB896DAC}"/>
   </bookViews>
@@ -45,169 +45,15 @@
     <t>thisY</t>
   </si>
   <si>
-    <r>
-      <t>Before we get started, here are some instructions!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Press any button to continue</t>
-    </r>
-  </si>
-  <si>
     <t>You will now complete a practice block of go trials</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Oops! That was a go trial </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you did not make a response!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Oops! That was a stop trial. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you did not withold </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>your response</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Correct!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> That was a Stop trial </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you withheld your response</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Correct! That was a go trial </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you made a response</t>
-    </r>
-  </si>
-  <si>
     <t>respKey</t>
   </si>
   <si>
     <t>Press and hold the {variable} key when you are ready!</t>
   </si>
   <si>
-    <t>Oops! You responded too soon!\n Press the {variable} key to restart countdown</t>
-  </si>
-  <si>
     <t>WrongKey - Please press the {variable} key</t>
   </si>
   <si>
@@ -244,9 +90,6 @@
     <t>practiceGoComplete</t>
   </si>
   <si>
-    <t>Great job. You have completed the practice block of go trials\n Do you understand the task?\n Please press (Y / N )</t>
-  </si>
-  <si>
     <t>testGoWarning</t>
   </si>
   <si>
@@ -259,12 +102,6 @@
     <t>practiceMixedComplete</t>
   </si>
   <si>
-    <t>Great job. You have completed the practice block of go and stop trials\n Do you understand the task?\n Please press (Y / N )</t>
-  </si>
-  <si>
-    <t>You will now complete a practice block of go and stop trials. \n Remember, on stop trials, if the bar stops before reaching the target,\n withhold your response until the arrows turn green!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Great job. You have completed a test block of go trials. </t>
   </si>
   <si>
@@ -274,66 +111,70 @@
     <t>testMixedWarning</t>
   </si>
   <si>
-    <r>
-      <t>You will now complete a test block of go trials</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Press space to continue</t>
-    </r>
-  </si>
-  <si>
     <t>doYouUnderstand</t>
   </si>
   <si>
-    <r>
-      <t>Do you understand the task</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Please press (Y / N)?</t>
-    </r>
-  </si>
-  <si>
     <t>almostGo</t>
   </si>
   <si>
-    <t>Try to stop the bar as close\n to the target as possible</t>
+    <t>Before we get started, here are some instructions!
+Press any button to continue</t>
+  </si>
+  <si>
+    <t>Great job. You have completed the practice block of go trials
+Do you understand the task?
+Please press (Y / N )</t>
+  </si>
+  <si>
+    <t>You will now complete a test block of go trials
+Press space to continue</t>
+  </si>
+  <si>
+    <t>You will now complete a practice block of go and stop trials.
+Remember, on stop trials, if the bar stops before reaching the target,
+withhold your response until the arrows turn green!</t>
+  </si>
+  <si>
+    <t>Great job. You have completed the practice block of go and stop trials
+Do you understand the task?
+Please press (Y / N )</t>
+  </si>
+  <si>
+    <t>Oops! You responded too soon!
+Press the {variable} key to restart countdown</t>
+  </si>
+  <si>
+    <t>Oops! That was a go trial 
+and you did not make a response!</t>
+  </si>
+  <si>
+    <t>Oops! That was a stop trial.
+and you did not withold
+your response</t>
+  </si>
+  <si>
+    <t>Correct! That was a go trial
+and you made a response</t>
+  </si>
+  <si>
+    <t>Do you understand the task
+Please press (Y / N)?</t>
+  </si>
+  <si>
+    <t>Try to stop the bar as close
+to the target as possible</t>
+  </si>
+  <si>
+    <t>Correct!
+That was a Stop trial
+and you withheld your response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,12 +185,6 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FFCC7832"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -380,13 +215,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5FFBA6-ED56-4ED1-AEF2-30899017D464}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -716,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -728,15 +566,15 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -750,10 +588,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -765,12 +603,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="39">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -782,12 +620,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="26">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -801,44 +639,44 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="39">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="39">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -852,10 +690,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -869,10 +707,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -884,12 +722,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="26">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C11">
         <v>-8</v>
@@ -901,12 +739,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="26">
       <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C12">
         <v>-8</v>
@@ -918,12 +756,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="39">
       <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C13">
         <v>-8</v>
@@ -935,12 +773,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="39">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C14">
         <v>-8</v>
@@ -954,10 +792,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>-8</v>
@@ -969,12 +807,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="26">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C16">
         <v>-8</v>
@@ -986,11 +824,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="26">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C17">
@@ -1003,12 +841,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="26">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C18">
         <v>-8</v>

</xml_diff>

<commit_message>
update input csv to be xlsx files
</commit_message>
<xml_diff>
--- a/conditionFiles/instructions.xlsx
+++ b/conditionFiles/instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Documents\GitHub\OSARI-1\conditionFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5274111C-BA24-4B28-ABAC-899D4163416E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FBBADD-596C-47DD-B119-FB240E33AE86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C4BCA8AB-96B2-4D72-9643-B068FB896DAC}"/>
   </bookViews>
@@ -33,6 +33,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={4655F973-2393-481D-B300-E77417F0B7E6}</author>
+    <author>tc={53015601-8BF7-4E91-B05C-F7B815C038F8}</author>
+    <author>tc={7D8EF187-8231-42EB-9C15-8BF6077DF831}</author>
+    <author>tc={80CDA7CE-37AB-41C1-852C-09B0F35A40E6}</author>
+    <author>tc={0DBF9722-D2E6-4006-980E-4B69B807E03F}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{4655F973-2393-481D-B300-E77417F0B7E6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    label for dictionary key used to call this instruction in OSARI.py</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{53015601-8BF7-4E91-B05C-F7B815C038F8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Text presented to participant in this instruction</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{7D8EF187-8231-42EB-9C15-8BF6077DF831}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The x coordinate of this instruction (in cm on screen units)</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{80CDA7CE-37AB-41C1-852C-09B0F35A40E6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The y coordinate of this instruction (in cm on screen units)</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{0DBF9722-D2E6-4006-980E-4B69B807E03F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Does this instruction need the response key included in it (inserted from experiment settings)</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
@@ -174,7 +228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,24 +237,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="9.8000000000000007"/>
-      <color theme="1"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,17 +280,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,6 +305,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="447975512226" id="{CD5D2A00-7D61-4A5B-A7BD-50BFC800979E}" userId="f6e9a7800afda06d" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,328 +608,349 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2021-04-18T09:38:07.01" personId="{CD5D2A00-7D61-4A5B-A7BD-50BFC800979E}" id="{4655F973-2393-481D-B300-E77417F0B7E6}">
+    <text>label for dictionary key used to call this instruction in OSARI.py</text>
+  </threadedComment>
+  <threadedComment ref="B1" dT="2021-04-18T09:38:26.30" personId="{CD5D2A00-7D61-4A5B-A7BD-50BFC800979E}" id="{53015601-8BF7-4E91-B05C-F7B815C038F8}">
+    <text>Text presented to participant in this instruction</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2021-04-18T09:38:48.98" personId="{CD5D2A00-7D61-4A5B-A7BD-50BFC800979E}" id="{7D8EF187-8231-42EB-9C15-8BF6077DF831}">
+    <text>The x coordinate of this instruction (in cm on screen units)</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2021-04-18T09:39:07.82" personId="{CD5D2A00-7D61-4A5B-A7BD-50BFC800979E}" id="{80CDA7CE-37AB-41C1-852C-09B0F35A40E6}">
+    <text>The y coordinate of this instruction (in cm on screen units)</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2021-04-18T09:40:33.07" personId="{CD5D2A00-7D61-4A5B-A7BD-50BFC800979E}" id="{0DBF9722-D2E6-4006-980E-4B69B807E03F}">
+    <text>Does this instruction need the response key included in it (inserted from experiment settings)</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5FFBA6-ED56-4ED1-AEF2-30899017D464}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5FFBA6-ED56-4ED1-AEF2-30899017D464}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.36328125" customWidth="1"/>
     <col min="2" max="2" width="121.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="39">
-      <c r="A4" t="s">
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="26">
-      <c r="A5" t="s">
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="39">
-      <c r="A7" t="s">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="39">
-      <c r="A8" t="s">
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="26">
-      <c r="A11" t="s">
+    <row r="11" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>-8</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="26">
-      <c r="A12" s="2" t="s">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>-8</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="39">
-      <c r="A13" s="2" t="s">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>-8</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="39">
-      <c r="A14" t="s">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>-8</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>-8</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="26">
-      <c r="A16" t="s">
+    <row r="16" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>-8</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="26">
-      <c r="A17" t="s">
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="26">
-      <c r="A18" t="s">
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>-8</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
import demographics from excel sheet
</commit_message>
<xml_diff>
--- a/conditionFiles/instructions.xlsx
+++ b/conditionFiles/instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\PycharmProjects\OSARI_private\conditionFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\Documents\GitHub\OSARI-1\conditionFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6931F62-CEEB-49C9-B4F3-B917764BC6F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5274111C-BA24-4B28-ABAC-899D4163416E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{C4BCA8AB-96B2-4D72-9643-B068FB896DAC}"/>
   </bookViews>
@@ -45,169 +45,15 @@
     <t>thisY</t>
   </si>
   <si>
-    <r>
-      <t>Before we get started, here are some instructions!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Press any button to continue</t>
-    </r>
-  </si>
-  <si>
     <t>You will now complete a practice block of go trials</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Oops! That was a go trial </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you did not make a response!</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Oops! That was a stop trial. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you did not withold </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>your response</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Correct!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> That was a Stop trial </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you withheld your response</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Correct! That was a go trial </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> and you made a response</t>
-    </r>
-  </si>
-  <si>
     <t>respKey</t>
   </si>
   <si>
     <t>Press and hold the {variable} key when you are ready!</t>
   </si>
   <si>
-    <t>Oops! You responded too soon!\n Press the {variable} key to restart countdown</t>
-  </si>
-  <si>
     <t>WrongKey - Please press the {variable} key</t>
   </si>
   <si>
@@ -244,9 +90,6 @@
     <t>practiceGoComplete</t>
   </si>
   <si>
-    <t>Great job. You have completed the practice block of go trials\n Do you understand the task?\n Please press (Y / N )</t>
-  </si>
-  <si>
     <t>testGoWarning</t>
   </si>
   <si>
@@ -259,12 +102,6 @@
     <t>practiceMixedComplete</t>
   </si>
   <si>
-    <t>Great job. You have completed the practice block of go and stop trials\n Do you understand the task?\n Please press (Y / N )</t>
-  </si>
-  <si>
-    <t>You will now complete a practice block of go and stop trials. \n Remember, on stop trials, if the bar stops before reaching the target,\n withhold your response until the arrows turn green!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Great job. You have completed a test block of go trials. </t>
   </si>
   <si>
@@ -274,66 +111,70 @@
     <t>testMixedWarning</t>
   </si>
   <si>
-    <r>
-      <t>You will now complete a test block of go trials</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Press space to continue</t>
-    </r>
-  </si>
-  <si>
     <t>doYouUnderstand</t>
   </si>
   <si>
-    <r>
-      <t>Do you understand the task</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FFCC7832"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>\n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.8000000000000007"/>
-        <color rgb="FF6A8759"/>
-        <rFont val="JetBrains Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve"> Please press (Y / N)?</t>
-    </r>
-  </si>
-  <si>
     <t>almostGo</t>
   </si>
   <si>
-    <t>Try to stop the bar as close\n to the target as possible</t>
+    <t>Before we get started, here are some instructions!
+Press any button to continue</t>
+  </si>
+  <si>
+    <t>Great job. You have completed the practice block of go trials
+Do you understand the task?
+Please press (Y / N )</t>
+  </si>
+  <si>
+    <t>You will now complete a test block of go trials
+Press space to continue</t>
+  </si>
+  <si>
+    <t>You will now complete a practice block of go and stop trials.
+Remember, on stop trials, if the bar stops before reaching the target,
+withhold your response until the arrows turn green!</t>
+  </si>
+  <si>
+    <t>Great job. You have completed the practice block of go and stop trials
+Do you understand the task?
+Please press (Y / N )</t>
+  </si>
+  <si>
+    <t>Oops! You responded too soon!
+Press the {variable} key to restart countdown</t>
+  </si>
+  <si>
+    <t>Oops! That was a go trial 
+and you did not make a response!</t>
+  </si>
+  <si>
+    <t>Oops! That was a stop trial.
+and you did not withold
+your response</t>
+  </si>
+  <si>
+    <t>Correct! That was a go trial
+and you made a response</t>
+  </si>
+  <si>
+    <t>Do you understand the task
+Please press (Y / N)?</t>
+  </si>
+  <si>
+    <t>Try to stop the bar as close
+to the target as possible</t>
+  </si>
+  <si>
+    <t>Correct!
+That was a Stop trial
+and you withheld your response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,12 +185,6 @@
     <font>
       <sz val="9.8000000000000007"/>
       <color rgb="FF6A8759"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="9.8000000000000007"/>
-      <color rgb="FFCC7832"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
@@ -380,13 +215,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -704,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5FFBA6-ED56-4ED1-AEF2-30899017D464}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -716,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -728,15 +566,15 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -750,10 +588,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -765,12 +603,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="39">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -782,12 +620,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="26">
       <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -801,44 +639,44 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="39">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="39">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -852,10 +690,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -869,10 +707,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -884,12 +722,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="26">
       <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C11">
         <v>-8</v>
@@ -901,12 +739,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" ht="26">
       <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C12">
         <v>-8</v>
@@ -918,12 +756,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="39">
       <c r="A13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C13">
         <v>-8</v>
@@ -935,12 +773,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="39">
       <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="C14">
         <v>-8</v>
@@ -954,10 +792,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>-8</v>
@@ -969,12 +807,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" ht="26">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C16">
         <v>-8</v>
@@ -986,11 +824,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" ht="26">
       <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C17">
@@ -1003,12 +841,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" ht="26">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="C18">
         <v>-8</v>

</xml_diff>